<commit_message>
change NLU file to separated with scenarios
</commit_message>
<xml_diff>
--- a/src/SmartKG.DataProcessor/Resources/_DataPreProcess/excel/Physics/SmartKG_KGDesc_PhonicsGrade7_zh.xlsx
+++ b/src/SmartKG.DataProcessor/Resources/_DataPreProcess/excel/Physics/SmartKG_KGDesc_PhonicsGrade7_zh.xlsx
@@ -1,21 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jull\source\repos\SmartKG\src\SmartKG.DataProcessor\Resources\_DataPreProcess\excel\Physics\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22E676D9-E9C1-4C00-8138-8FB236DF813C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vertexes" sheetId="1" r:id="rId1"/>
     <sheet name="Edges" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="79">
   <si>
     <t>实体id</t>
   </si>
@@ -243,13 +249,22 @@
   </si>
   <si>
     <t>包含</t>
+  </si>
+  <si>
+    <t>概念</t>
+  </si>
+  <si>
+    <t>行为</t>
+  </si>
+  <si>
+    <t>属性</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -286,6 +301,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -332,7 +355,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -364,9 +387,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -398,6 +439,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -573,14 +632,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="19.3984375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -618,24 +682,30 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>15</v>
       </c>
+      <c r="C2" t="s">
+        <v>76</v>
+      </c>
       <c r="D2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>16</v>
       </c>
+      <c r="C3" t="s">
+        <v>77</v>
+      </c>
       <c r="E3" t="s">
         <v>32</v>
       </c>
@@ -643,13 +713,16 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>17</v>
       </c>
+      <c r="C4" t="s">
+        <v>77</v>
+      </c>
       <c r="E4" t="s">
         <v>33</v>
       </c>
@@ -669,24 +742,30 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>18</v>
       </c>
+      <c r="C5" t="s">
+        <v>78</v>
+      </c>
       <c r="D5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>19</v>
       </c>
+      <c r="C6" t="s">
+        <v>76</v>
+      </c>
       <c r="E6" t="s">
         <v>34</v>
       </c>
@@ -706,13 +785,16 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>20</v>
       </c>
+      <c r="C7" t="s">
+        <v>76</v>
+      </c>
       <c r="E7" t="s">
         <v>34</v>
       </c>
@@ -726,13 +808,16 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>21</v>
       </c>
+      <c r="C8" t="s">
+        <v>76</v>
+      </c>
       <c r="E8" t="s">
         <v>34</v>
       </c>
@@ -746,24 +831,30 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>22</v>
       </c>
+      <c r="C9" t="s">
+        <v>77</v>
+      </c>
       <c r="D9" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>23</v>
       </c>
+      <c r="C10" t="s">
+        <v>77</v>
+      </c>
       <c r="E10" t="s">
         <v>35</v>
       </c>
@@ -771,13 +862,16 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>24</v>
       </c>
+      <c r="C11" t="s">
+        <v>77</v>
+      </c>
       <c r="E11" t="s">
         <v>35</v>
       </c>
@@ -785,24 +879,30 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>25</v>
       </c>
+      <c r="C12" t="s">
+        <v>78</v>
+      </c>
       <c r="D12" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>26</v>
       </c>
+      <c r="C13" t="s">
+        <v>76</v>
+      </c>
       <c r="E13" t="s">
         <v>36</v>
       </c>
@@ -816,12 +916,15 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>13</v>
       </c>
       <c r="B14" t="s">
         <v>27</v>
+      </c>
+      <c r="C14" t="s">
+        <v>76</v>
       </c>
       <c r="E14" t="s">
         <v>36</v>
@@ -860,14 +963,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="30.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>72</v>
       </c>
@@ -878,7 +984,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>75</v>
       </c>
@@ -889,7 +995,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>75</v>
       </c>
@@ -900,7 +1006,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>75</v>
       </c>
@@ -911,7 +1017,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>75</v>
       </c>
@@ -922,7 +1028,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>75</v>
       </c>
@@ -933,7 +1039,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>75</v>
       </c>
@@ -944,7 +1050,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>75</v>
       </c>
@@ -955,7 +1061,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>75</v>
       </c>
@@ -966,7 +1072,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>75</v>
       </c>
@@ -977,7 +1083,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>75</v>
       </c>
@@ -988,7 +1094,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>75</v>
       </c>
@@ -999,7 +1105,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>75</v>
       </c>

</xml_diff>